<commit_message>
only issue on another suite, it lost data
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite.xlsx
+++ b/src/main/resources/project/Suite.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
-    <t>Scenario: Test Suite</t>
+    <t>Scenario: Scenario</t>
   </si>
   <si>
     <t>Item</t>
@@ -77,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -122,6 +122,40 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>